<commit_message>
all core strat added plus the source header.
</commit_message>
<xml_diff>
--- a/strats-sources/common_proto.xlsx
+++ b/strats-sources/common_proto.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\gitrepos\w40k-strat-card\strats-sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5284D5-A449-4BD3-A1B8-8F3D0609C4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DE4184-7E91-41EC-B354-78234FA2FEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="2655" windowWidth="19695" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>StratScreenshot</t>
   </si>
@@ -36,25 +47,76 @@
     <t>Relance de Commandement</t>
   </si>
   <si>
-    <t>strats-sources\assets\v10_screenshots\00_Core_RelanceCommandement.png</t>
-  </si>
-  <si>
     <t>Contre Offensive</t>
   </si>
   <si>
-    <t>strats-sources\assets\v10_screenshots\01_Core_ContreOffensive.png</t>
-  </si>
-  <si>
     <t>Defi Epique</t>
   </si>
   <si>
-    <t>strats-sources\assets\v10_screenshots\02_Core_DefiEpique.png</t>
-  </si>
-  <si>
-    <t>strats-sources\assets\v10_screenshots\03_Core_CourageInsense.png</t>
-  </si>
-  <si>
     <t>Courage Insense</t>
+  </si>
+  <si>
+    <t>Attaque de Char</t>
+  </si>
+  <si>
+    <t>RelativePath</t>
+  </si>
+  <si>
+    <t>strats-sources\assets\v10_screenshots</t>
+  </si>
+  <si>
+    <t>00_Core_RelanceCommandement.png</t>
+  </si>
+  <si>
+    <t>01_Core_ContreOffensive.png</t>
+  </si>
+  <si>
+    <t>02_Core_DefiEpique.png</t>
+  </si>
+  <si>
+    <t>03_Core_CourageInsense.png</t>
+  </si>
+  <si>
+    <t>04_Core_Grenade.png</t>
+  </si>
+  <si>
+    <t>05_Core_AttaqueDeChar.png</t>
+  </si>
+  <si>
+    <t>06_Core_TirEtatAlerte.png</t>
+  </si>
+  <si>
+    <t>07_Core_ArriveePrecipitee.png</t>
+  </si>
+  <si>
+    <t>08_Core_ATerre.png</t>
+  </si>
+  <si>
+    <t>09_Core_EcranFumee.png</t>
+  </si>
+  <si>
+    <t>10_Core_InterventionHeroique.png</t>
+  </si>
+  <si>
+    <t>Tir en Etat d'alerte</t>
+  </si>
+  <si>
+    <t>Arrivee precipitee</t>
+  </si>
+  <si>
+    <t>A Terre</t>
+  </si>
+  <si>
+    <t>Ecran de Fumee</t>
+  </si>
+  <si>
+    <t>Intervention Heroique</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Core</t>
   </si>
 </sst>
 </file>
@@ -372,55 +434,229 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="str">
+        <f>(E2 &amp; "\" &amp; D2)</f>
+        <v>strats-sources\assets\v10_screenshots\00_Core_RelanceCommandement.png</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C12" si="0">(E3 &amp; "\" &amp; D3)</f>
+        <v>strats-sources\assets\v10_screenshots\01_Core_ContreOffensive.png</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>strats-sources\assets\v10_screenshots\02_Core_DefiEpique.png</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>strats-sources\assets\v10_screenshots\03_Core_CourageInsense.png</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>strats-sources\assets\v10_screenshots\04_Core_Grenade.png</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>strats-sources\assets\v10_screenshots\05_Core_AttaqueDeChar.png</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>strats-sources\assets\v10_screenshots\06_Core_TirEtatAlerte.png</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>strats-sources\assets\v10_screenshots\07_Core_ArriveePrecipitee.png</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>strats-sources\assets\v10_screenshots\08_Core_ATerre.png</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>strats-sources\assets\v10_screenshots\09_Core_EcranFumee.png</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>strats-sources\assets\v10_screenshots\10_Core_InterventionHeroique.png</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added blood angel strats.
</commit_message>
<xml_diff>
--- a/strats-sources/common_proto.xlsx
+++ b/strats-sources/common_proto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\gitrepos\w40k-strat-card\strats-sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594CBFDD-D014-44BC-AB37-2957E1650AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FB99E9-85D6-4A98-90E5-6C99BDA8799A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7680" yWindow="2655" windowWidth="19695" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t>StratScreenshot</t>
   </si>
@@ -117,12 +117,69 @@
   </si>
   <si>
     <t>Core</t>
+  </si>
+  <si>
+    <t>UpdateDate</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>BloodAngel_00_SacrificeDelAnge.png</t>
+  </si>
+  <si>
+    <t>BloodAngel_01_ArmureDuMepris.png</t>
+  </si>
+  <si>
+    <t>BloodAngel_02_OffenseiveAgressive.png</t>
+  </si>
+  <si>
+    <t>BloodAngel_03_CarnageRouge.png</t>
+  </si>
+  <si>
+    <t>BloodAngel_04_SeuleLaMort.png</t>
+  </si>
+  <si>
+    <t>BloodAngel_05_AssautImplacable.png</t>
+  </si>
+  <si>
+    <t>Sacrifice de l'Ange</t>
+  </si>
+  <si>
+    <t>Armure du Mepris</t>
+  </si>
+  <si>
+    <t>Offensive Aggressive</t>
+  </si>
+  <si>
+    <t>Carnage Rouge</t>
+  </si>
+  <si>
+    <t>Seule la mort mets fin au Devoir</t>
+  </si>
+  <si>
+    <t>SerieCardNumber</t>
+  </si>
+  <si>
+    <t>SerieTotalCardNumber</t>
+  </si>
+  <si>
+    <t>Assaut Implacable</t>
+  </si>
+  <si>
+    <t>Blood Angel</t>
+  </si>
+  <si>
+    <t>TotalCardId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -152,8 +209,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,233 +492,635 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C26" sqref="C25:C26"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.85546875" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="71.85546875" customWidth="1"/>
+    <col min="10" max="10" width="35.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>11</v>
+      </c>
+      <c r="F2" t="str">
+        <f>_xlfn.CONCAT(D2 &amp; "/" &amp; E2)</f>
+        <v>1/11</v>
+      </c>
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="str">
-        <f>(E2 &amp; "\" &amp; D2)</f>
+      <c r="H2" t="str">
+        <f>(J2 &amp; "\" &amp; I2)</f>
         <v>strats-sources\assets\v10_screenshots\00_Core_RelanceCommandement.png</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F18" si="0">_xlfn.CONCAT(D3 &amp; "/" &amp; E3)</f>
+        <v>2/11</v>
+      </c>
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C12" si="0">(E3 &amp; "\" &amp; D3)</f>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H18" si="1">(J3 &amp; "\" &amp; I3)</f>
         <v>strats-sources\assets\v10_screenshots\01_Core_ContreOffensive.png</v>
       </c>
-      <c r="D3" t="s">
+      <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>11</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>3/11</v>
+      </c>
+      <c r="G4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
         <v>strats-sources\assets\v10_screenshots\02_Core_DefiEpique.png</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>11</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>4/11</v>
+      </c>
+      <c r="G5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
         <v>strats-sources\assets\v10_screenshots\03_Core_CourageInsense.png</v>
       </c>
-      <c r="D5" t="s">
+      <c r="I5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>5/11</v>
+      </c>
+      <c r="G6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
         <v>strats-sources\assets\v10_screenshots\04_Core_Grenade.png</v>
       </c>
-      <c r="D6" t="s">
+      <c r="I6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>11</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>6/11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
         <v>strats-sources\assets\v10_screenshots\05_Core_AttaqueDeChar.png</v>
       </c>
-      <c r="D7" t="s">
+      <c r="I7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>11</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>7/11</v>
+      </c>
+      <c r="G8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
         <v>strats-sources\assets\v10_screenshots\06_Core_TirEtatAlerte.png</v>
       </c>
-      <c r="D8" t="s">
+      <c r="I8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>11</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>8/11</v>
+      </c>
+      <c r="G9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
         <v>strats-sources\assets\v10_screenshots\07_Core_ArriveePrecipitee.png</v>
       </c>
-      <c r="D9" t="s">
+      <c r="I9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>9/11</v>
+      </c>
+      <c r="G10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="str">
-        <f t="shared" si="0"/>
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
         <v>strats-sources\assets\v10_screenshots\08_Core_ATerre.png</v>
       </c>
-      <c r="D10" t="s">
+      <c r="I10" t="s">
         <v>17</v>
       </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="J10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>10/11</v>
+      </c>
+      <c r="G11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="str">
-        <f t="shared" si="0"/>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
         <v>strats-sources\assets\v10_screenshots\09_Core_EcranFumee.png</v>
       </c>
-      <c r="D11" t="s">
+      <c r="I11" t="s">
         <v>18</v>
       </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="J11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>11/11</v>
+      </c>
+      <c r="G12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="str">
-        <f t="shared" si="0"/>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
         <v>strats-sources\assets\v10_screenshots\10_Core_InterventionHeroique.png</v>
       </c>
-      <c r="D12" t="s">
+      <c r="I12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" t="s">
+      <c r="J12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>1/6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>strats-sources\assets\v10_screenshots\BloodAngel_00_SacrificeDelAnge.png</v>
+      </c>
+      <c r="I13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>6</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>2/6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>strats-sources\assets\v10_screenshots\BloodAngel_01_ArmureDuMepris.png</v>
+      </c>
+      <c r="I14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>3/6</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>strats-sources\assets\v10_screenshots\BloodAngel_02_OffenseiveAgressive.png</v>
+      </c>
+      <c r="I15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>4/6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>strats-sources\assets\v10_screenshots\BloodAngel_03_CarnageRouge.png</v>
+      </c>
+      <c r="I16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>5/6</v>
+      </c>
+      <c r="G17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
+        <v>strats-sources\assets\v10_screenshots\BloodAngel_04_SeuleLaMort.png</v>
+      </c>
+      <c r="I17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>6</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>6/6</v>
+      </c>
+      <c r="G18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v>strats-sources\assets\v10_screenshots\BloodAngel_05_AssautImplacable.png</v>
+      </c>
+      <c r="I18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>